<commit_message>
Kalibrering med IO data i Jonathan
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/IOdata_dors_2.xlsx
+++ b/examples/Abatement/Data/IOdata_dors_2.xlsx
@@ -382,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,13 +410,13 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -424,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -432,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,7 +440,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -456,7 +456,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>